<commit_message>
Mejoras, se agregan ejemplos de los otros cursos
</commit_message>
<xml_diff>
--- a/ApiWebCucumberFrameworkMaster/src/main/java/resources/TestData/testdata.xlsx
+++ b/ApiWebCucumberFrameworkMaster/src/main/java/resources/TestData/testdata.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="compradores" sheetId="1" r:id="rId1"/>
+    <sheet name="apidata" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,12 +19,88 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+  <si>
+    <t>comprador1</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>apellido</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Giulio</t>
+  </si>
+  <si>
+    <t>Faragalli</t>
+  </si>
+  <si>
+    <t>GFemail@email.com</t>
+  </si>
+  <si>
+    <t>genero</t>
+  </si>
+  <si>
+    <t>masculino</t>
+  </si>
+  <si>
+    <t>dataKey</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>place1</t>
+  </si>
+  <si>
+    <t>place2</t>
+  </si>
+  <si>
+    <t>AAhouse</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>World cross center</t>
+  </si>
+  <si>
+    <t>BBhouse</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Sea cross center</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +123,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -69,7 +149,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +194,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +229,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +411,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>